<commit_message>
git commit -m "finish logo"
</commit_message>
<xml_diff>
--- a/프로젝트.xlsx
+++ b/프로젝트.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tech stack" sheetId="2" r:id="rId1"/>
     <sheet name="blueprint" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="idea" sheetId="4" r:id="rId3"/>
     <sheet name="DB" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>메뉴 id, 메뉴 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>medibang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강제성을 부여하기 위해 추가되어야 할 것?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마일리지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식습관 정보 + 건강</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,15 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -481,6 +484,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -824,22 +836,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="8" customWidth="1"/>
+    <col min="1" max="1" width="6.69921875" style="8" customWidth="1"/>
     <col min="2" max="2" width="12" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:3" ht="19.2" x14ac:dyDescent="0.45">
+      <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -850,7 +862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -861,7 +873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -872,7 +884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -883,7 +895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -891,32 +903,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B15" s="8" t="s">
         <v>68</v>
       </c>
@@ -935,196 +947,196 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9" style="17"/>
-    <col min="2" max="2" width="9" style="15"/>
-    <col min="3" max="3" width="11.25" style="17" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="17"/>
+    <col min="1" max="1" width="9" style="14"/>
+    <col min="2" max="2" width="9" style="12"/>
+    <col min="3" max="3" width="11.19921875" style="14" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C5" s="16"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="17"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="16"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C8" s="16"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="16" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C9" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="15">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B13" s="12">
         <v>1</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="16" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="17" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C15" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="17" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C16" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C17" s="17" t="s">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="C17" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="15">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B19" s="12">
         <v>2</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M19" s="17" t="s">
+      <c r="M19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="17" t="s">
+      <c r="N19" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="R19" s="17" t="s">
+      <c r="R19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="S19" s="17" t="s">
+      <c r="S19" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C20" s="16" t="s">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="C20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="H20" s="17" t="s">
+      <c r="F20" s="15"/>
+      <c r="H20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="N20" s="17" t="s">
+      <c r="N20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="S20" s="17" t="s">
+      <c r="S20" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C21" s="16" t="s">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="C21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="17" t="s">
+      <c r="N21" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C22" s="16" t="s">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="C22" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="17" t="s">
+      <c r="N22" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="15" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B40" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="15" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B41" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="15" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B42" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="15" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B43" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="15" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B44" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="15" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B45" s="12" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1138,40 +1150,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C9:S20"/>
+  <dimension ref="C9:S22"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.4">
       <c r="G13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:19" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="R19" s="14">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.4">
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="R19" s="11">
         <v>44960</v>
       </c>
       <c r="S19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.4">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
       <c r="S20" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.4">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.4">
+      <c r="C22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1188,21 +1222,21 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" customWidth="1"/>
     <col min="5" max="5" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+    <row r="3" spans="3:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C5" s="5">
         <v>1</v>
       </c>
@@ -1213,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C6" s="5">
         <v>2</v>
       </c>
@@ -1224,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C7" s="5">
         <v>3</v>
       </c>
@@ -1235,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C8" s="5">
         <v>4</v>
       </c>
@@ -1246,7 +1280,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C9" s="9" t="s">
         <v>66</v>
       </c>
@@ -1257,29 +1291,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="G13" t="s">
         <v>60</v>
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="10" t="s">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C15" s="5">
         <v>1</v>
       </c>
@@ -1290,28 +1324,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:19" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.4">
       <c r="C19" s="5"/>
       <c r="D19" s="7"/>
       <c r="E19" s="2"/>
-      <c r="R19" s="14">
+      <c r="R19" s="11">
         <v>44960</v>
       </c>
       <c r="S19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
       <c r="D20" s="7"/>
       <c r="E20" s="2"/>
@@ -1319,12 +1353,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="3:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C22" s="6"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>

</xml_diff>